<commit_message>
New auction admin side
</commit_message>
<xml_diff>
--- a/src/main/resources/auction_unit.xlsx
+++ b/src/main/resources/auction_unit.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\SaknaiNewEnv\SAKANI_TST_NEW\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\SAKANI_NEW_TST\SAKANI_TST_R1_IBR\SAKANI_TST_R1\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BC4A78-81DC-49BE-9C9C-100205BD3B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28049B81-A2D4-471B-8080-41451202FA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="100">
   <si>
     <t>رقم البلوك / Block Number</t>
   </si>
@@ -317,28 +317,25 @@
     <t>الجنسية / Nationality</t>
   </si>
   <si>
-    <t>1446-6-22</t>
+    <t>10:51</t>
   </si>
   <si>
-    <t>14:00</t>
+    <t>10:35</t>
   </si>
   <si>
-    <t>15:00</t>
+    <t>1441-1-14</t>
   </si>
   <si>
-    <t>1446-06-23</t>
+    <t>1446-06-24</t>
   </si>
   <si>
-    <t>10:00</t>
+    <t>10:41</t>
   </si>
   <si>
-    <t>11:00</t>
+    <t>1446-6-24</t>
   </si>
   <si>
-    <t>06:00</t>
-  </si>
-  <si>
-    <t>09:00</t>
+    <t>10:49</t>
   </si>
 </sst>
 </file>
@@ -1623,7 +1620,7 @@
   <dimension ref="A1:BV284"/>
   <sheetViews>
     <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" topLeftCell="AT1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="AZ2" sqref="AZ2"/>
+      <selection activeCell="AZ12" sqref="AZ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1999,16 +1996,16 @@
         <v>78</v>
       </c>
       <c r="AZ2" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="BA2" s="5" t="s">
         <v>99</v>
       </c>
       <c r="BB2" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="BC2" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="BD2" s="5" t="s">
         <v>90</v>

</xml_diff>